<commit_message>
New IV and DVs
Density changed and abs-performance. Also changed renv
</commit_message>
<xml_diff>
--- a/MLR_variables.xlsx
+++ b/MLR_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcmel/Documents/PhD/Papers/07 Lana ECPR paper/stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C47401-7A3E-984B-8CC7-43C530307D10}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B124D6BC-60F6-F04F-BEB8-691EA8DDE007}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{6BD1A52F-6E32-C94B-8F17-FD9EAF1BC1AF}"/>
+    <workbookView xWindow="0" yWindow="1460" windowWidth="28800" windowHeight="16240" xr2:uid="{6BD1A52F-6E32-C94B-8F17-FD9EAF1BC1AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="108">
   <si>
     <t>EE.perfor.</t>
   </si>
@@ -81,9 +81,6 @@
     <t>P_density</t>
   </si>
   <si>
-    <t xml:space="preserve">performance on NREAP </t>
-  </si>
-  <si>
     <t>mean_progress_NREAP</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>subsidies_REN</t>
   </si>
   <si>
-    <t>Policy_density_REN</t>
-  </si>
-  <si>
     <t>renewed_mean_progress_linear_trajectory</t>
   </si>
   <si>
@@ -111,9 +105,6 @@
     <t>col_names_for_EE</t>
   </si>
   <si>
-    <t>Policy_density_EE</t>
-  </si>
-  <si>
     <t>subsidies_savings</t>
   </si>
   <si>
@@ -198,15 +189,9 @@
     <t>Target Ambition (NEEAP/NREAP)</t>
   </si>
   <si>
-    <t>performance on NEEAP</t>
-  </si>
-  <si>
     <t>Policy density</t>
   </si>
   <si>
-    <t>Percentage of instruments implemented to promote energy efficiency/renewable energy in the field of climate mitigation</t>
-  </si>
-  <si>
     <t>(Over/under)- performance towards 2020 targets in the 2017 NREAP, as the mean difference of 2016-2018  trajectory( assuming a linear trajectory between 2005 and 2020).</t>
   </si>
   <si>
@@ -325,6 +310,45 @@
   </si>
   <si>
     <t>Size of the services</t>
+  </si>
+  <si>
+    <t>EE_policies</t>
+  </si>
+  <si>
+    <t>REN_policies</t>
+  </si>
+  <si>
+    <t>Number of policies</t>
+  </si>
+  <si>
+    <t>EE_perf_abs</t>
+  </si>
+  <si>
+    <t>absolute_progress_EE</t>
+  </si>
+  <si>
+    <t>absolute_progress_REN</t>
+  </si>
+  <si>
+    <t>EE.perfor.abs</t>
+  </si>
+  <si>
+    <t>REN.perfor.abs</t>
+  </si>
+  <si>
+    <t>Absolute performance on NREAP</t>
+  </si>
+  <si>
+    <t>Absolute performance on NEEAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relative performance on NREAP </t>
+  </si>
+  <si>
+    <t>Relative performance on NEEAP</t>
+  </si>
+  <si>
+    <t>RE_perf_abs</t>
   </si>
 </sst>
 </file>
@@ -340,12 +364,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -360,9 +390,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FBA15E7-0942-7F4F-B708-FE900CBE0D04}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="183" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="183" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -695,31 +726,31 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -727,16 +758,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -745,7 +776,7 @@
         <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -753,16 +784,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
         <v>60</v>
-      </c>
-      <c r="D3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" t="s">
-        <v>65</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
@@ -771,172 +802,154 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" t="s">
-        <v>65</v>
+        <v>98</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" t="s">
-        <v>84</v>
+        <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" t="s">
-        <v>59</v>
+        <v>103</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>65</v>
+        <v>107</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>3</v>
+        <v>102</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="J6" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" t="s">
-        <v>65</v>
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="G7" t="s">
         <v>16</v>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I7" t="s">
-        <v>22</v>
+        <v>96</v>
       </c>
       <c r="J7" t="s">
-        <v>30</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>68</v>
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>60</v>
       </c>
       <c r="F8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G8" t="s">
         <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>49</v>
@@ -945,13 +958,13 @@
         <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F9" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G9" t="s">
         <v>16</v>
@@ -960,30 +973,30 @@
         <v>10</v>
       </c>
       <c r="I9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G10" t="s">
         <v>16</v>
@@ -992,30 +1005,30 @@
         <v>10</v>
       </c>
       <c r="I10" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="J10" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G11" t="s">
         <v>16</v>
@@ -1024,30 +1037,30 @@
         <v>10</v>
       </c>
       <c r="I11" t="s">
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="J11" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" t="s">
-        <v>65</v>
+        <v>13</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="F12" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="G12" t="s">
         <v>16</v>
@@ -1056,62 +1069,62 @@
         <v>10</v>
       </c>
       <c r="I12" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="J12" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="F13" t="s">
-        <v>79</v>
+        <v>9</v>
       </c>
       <c r="G13" t="s">
         <v>16</v>
       </c>
       <c r="H13" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I13" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="J13" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="D14" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F14" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="G14" t="s">
         <v>16</v>
@@ -1120,56 +1133,62 @@
         <v>10</v>
       </c>
       <c r="I14" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="J14" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="E15" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="F15" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="G15" t="s">
         <v>16</v>
       </c>
       <c r="H15" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I15" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="J15" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>98</v>
+        <v>76</v>
+      </c>
+      <c r="C16" t="s">
+        <v>75</v>
       </c>
       <c r="D16" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="F16" t="s">
+        <v>77</v>
       </c>
       <c r="G16" t="s">
         <v>16</v>
@@ -1178,24 +1197,30 @@
         <v>10</v>
       </c>
       <c r="I16" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="J16" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>99</v>
+        <v>88</v>
+      </c>
+      <c r="C17" t="s">
+        <v>86</v>
       </c>
       <c r="D17" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="F17" t="s">
+        <v>85</v>
       </c>
       <c r="G17" t="s">
         <v>16</v>
@@ -1204,10 +1229,62 @@
         <v>10</v>
       </c>
       <c r="I17" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="J17" t="s">
-        <v>95</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" t="s">
+        <v>89</v>
+      </c>
+      <c r="J18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" t="s">
+        <v>90</v>
+      </c>
+      <c r="J19" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>